<commit_message>
updated test list list & added missing test cases in DV Plans
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/debug-trace/CV32E40Pv2_debug.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/debug-trace/CV32E40Pv2_debug.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\debug-trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99EFFEB-3E80-4897-A568-6553BAF300B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C818E4-5551-40C4-8CB2-25339A3A62E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="5250" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="259">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -3070,11 +3070,6 @@
 corev_rand_pulp_instr_interrupt_debug_test</t>
   </si>
   <si>
-    <t>corev_rand_pulp_instr_debug_trigger_with_random_debug_req
-corev_rand_pulp_instr_debug_ebreak_with_random_debug_req
-corev_rand_pulp_instr_debug_single_step_with_random_debug_req</t>
-  </si>
-  <si>
     <t>N/A: Hard to detect that we are executing an exception handler.
 Covered in debug_test with RM enabled.</t>
   </si>
@@ -3213,9 +3208,6 @@
     <t>A:   uvmt_cv32_tb.u_debug_assert.a_dmode_dret</t>
   </si>
   <si>
-    <t>corev_rand_pulp_instr_debug_test_with_int_and_debug_single_step</t>
-  </si>
-  <si>
     <t>corev_rand_pulp_instr_interrupt_debug_test</t>
   </si>
   <si>
@@ -3223,10 +3215,6 @@
   </si>
   <si>
     <t>corev_rand_pulp_instr_debug_trigger_with_single_step</t>
-  </si>
-  <si>
-    <t>corev_rand_debug_single_step
-corev_rand_debug_single_step_xpulp</t>
   </si>
   <si>
     <t xml:space="preserve">debug_test
@@ -3240,18 +3228,47 @@
   <si>
     <t>corev_rand_pulp_instr_debug_trigger_with_random_debug_req</t>
   </si>
+  <si>
+    <t>corev_rand_pulp_instr_debug_trigger_with_ebreak
+corev_rand_pulp_instr_debug_trigger_with_single_step
+corev_rand_pulp_instr_debug_trigger_with_random_debug_req
+corev_rand_pulp_instr_debug_ebreak_with_random_debug_req
+corev_rand_pulp_instr_debug_single_step_with_random_debug_req</t>
+  </si>
+  <si>
+    <t>corev_rand_pulp_instr_debug_test_with_int_and_debug_single_step
+corev_rand_fp_instr_debug_test_with_int_and_debug_single_step
+corev_rand_fp_instr_debug_test_with_int_debug_trigger_and_single_step</t>
+  </si>
+  <si>
+    <t>corev_rand_debug_single_step
+corev_rand_debug_single_step_xpulp
+corev_rand_pulp_instr_single_step_debug_test</t>
+  </si>
+  <si>
+    <t>corev_rand_debug_ebreak
+corev_rand_debug_ebreak_xpulp
+corev_rand_pulp_instr_ebreak_debug_test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3587,78 +3604,131 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3666,20 +3736,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3687,63 +3755,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{1E1B0CF8-8C4F-41A9-9558-CBA9FC1B75F5}"/>
@@ -4236,9 +4259,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AMV137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4314,22 +4337,22 @@
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="1:21" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="43" t="s">
         <v>128</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -4359,12 +4382,12 @@
       <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:21" s="4" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
       <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
@@ -4381,7 +4404,7 @@
         <v>207</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N3"/>
       <c r="O3"/>
@@ -4392,12 +4415,12 @@
       <c r="U3" s="13"/>
     </row>
     <row r="4" spans="1:21" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4414,7 +4437,7 @@
         <v>207</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N4"/>
       <c r="O4"/>
@@ -4425,22 +4448,22 @@
       <c r="U4" s="13"/>
     </row>
     <row r="5" spans="1:21" s="4" customFormat="1" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="43" t="s">
         <v>134</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -4470,12 +4493,12 @@
       <c r="T5" s="21"/>
     </row>
     <row r="6" spans="1:21" s="4" customFormat="1" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
@@ -4492,7 +4515,7 @@
         <v>191</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N6"/>
       <c r="O6"/>
@@ -4502,10 +4525,10 @@
       <c r="S6"/>
     </row>
     <row r="7" spans="1:21" s="4" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="43" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -4548,8 +4571,8 @@
       <c r="U7" s="13"/>
     </row>
     <row r="8" spans="1:21" s="4" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
       <c r="E8" s="45"/>
@@ -4570,7 +4593,7 @@
         <v>207</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N8"/>
       <c r="O8"/>
@@ -4582,8 +4605,8 @@
       <c r="U8" s="13"/>
     </row>
     <row r="9" spans="1:21" s="4" customFormat="1" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
       <c r="E9" s="45"/>
@@ -4604,7 +4627,7 @@
         <v>207</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N9"/>
       <c r="O9"/>
@@ -4615,10 +4638,10 @@
       <c r="U9" s="13"/>
     </row>
     <row r="10" spans="1:21" s="3" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="43" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="46" t="s">
@@ -4662,8 +4685,8 @@
       <c r="U10" s="13"/>
     </row>
     <row r="11" spans="1:21" s="3" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="46"/>
       <c r="D11" s="44"/>
       <c r="E11" s="45"/>
@@ -4684,7 +4707,7 @@
         <v>207</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11"/>
@@ -4697,8 +4720,8 @@
       <c r="U11" s="13"/>
     </row>
     <row r="12" spans="1:21" s="3" customFormat="1" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
       <c r="E12" s="45"/>
@@ -4719,7 +4742,7 @@
         <v>207</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12"/>
@@ -4732,22 +4755,22 @@
       <c r="U12" s="13"/>
     </row>
     <row r="13" spans="1:21" s="3" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="51" t="s">
         <v>131</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -4778,12 +4801,12 @@
       <c r="U13" s="13"/>
     </row>
     <row r="14" spans="1:21" s="3" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="5" t="s">
         <v>12</v>
       </c>
@@ -4800,7 +4823,7 @@
         <v>208</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14"/>
@@ -4812,12 +4835,12 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:21" s="3" customFormat="1" ht="175.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
@@ -4834,7 +4857,7 @@
         <v>208</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15"/>
@@ -4846,22 +4869,22 @@
       <c r="U15" s="13"/>
     </row>
     <row r="16" spans="1:21" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="43" t="s">
         <v>108</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -4890,12 +4913,12 @@
       <c r="S16"/>
     </row>
     <row r="17" spans="1:21" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
@@ -4911,8 +4934,8 @@
       <c r="K17" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L17" s="50" t="s">
-        <v>223</v>
+      <c r="L17" s="33" t="s">
+        <v>222</v>
       </c>
       <c r="N17"/>
       <c r="O17"/>
@@ -4922,12 +4945,12 @@
       <c r="S17"/>
     </row>
     <row r="18" spans="1:21" s="3" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
       <c r="G18" s="5" t="s">
         <v>12</v>
       </c>
@@ -4944,7 +4967,7 @@
         <v>208</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N18"/>
       <c r="O18"/>
@@ -4954,22 +4977,22 @@
       <c r="S18"/>
     </row>
     <row r="19" spans="1:21" s="3" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="41" t="s">
         <v>136</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -4998,12 +5021,12 @@
       <c r="U19" s="13"/>
     </row>
     <row r="20" spans="1:21" s="3" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="5" t="s">
         <v>12</v>
       </c>
@@ -5019,8 +5042,8 @@
       <c r="K20" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L20" s="50" t="s">
-        <v>225</v>
+      <c r="L20" s="33" t="s">
+        <v>224</v>
       </c>
       <c r="O20"/>
       <c r="P20"/>
@@ -5030,12 +5053,12 @@
       <c r="U20" s="13"/>
     </row>
     <row r="21" spans="1:21" s="3" customFormat="1" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="5" t="s">
         <v>12</v>
       </c>
@@ -5052,7 +5075,7 @@
         <v>208</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21"/>
@@ -5063,20 +5086,20 @@
       <c r="U21" s="13"/>
     </row>
     <row r="22" spans="1:21" s="3" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35" t="s">
+      <c r="D22" s="43"/>
+      <c r="E22" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="43" t="s">
         <v>104</v>
       </c>
       <c r="G22" s="5" t="s">
@@ -5106,12 +5129,12 @@
       <c r="U22" s="13"/>
     </row>
     <row r="23" spans="1:21" s="3" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
       <c r="G23" s="5" t="s">
         <v>12</v>
       </c>
@@ -5125,8 +5148,8 @@
         <v>21</v>
       </c>
       <c r="K23" s="5"/>
-      <c r="L23" s="50" t="s">
-        <v>227</v>
+      <c r="L23" s="33" t="s">
+        <v>226</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -5137,12 +5160,12 @@
       <c r="U23" s="13"/>
     </row>
     <row r="24" spans="1:21" s="3" customFormat="1" ht="90.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
       <c r="G24" s="5" t="s">
         <v>12</v>
       </c>
@@ -5156,8 +5179,8 @@
         <v>22</v>
       </c>
       <c r="K24" s="5"/>
-      <c r="L24" s="50" t="s">
-        <v>226</v>
+      <c r="L24" s="33" t="s">
+        <v>225</v>
       </c>
       <c r="N24"/>
       <c r="O24"/>
@@ -5168,20 +5191,20 @@
       <c r="U24" s="13"/>
     </row>
     <row r="25" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35" t="s">
+      <c r="D25" s="43"/>
+      <c r="E25" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="43" t="s">
         <v>40</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -5211,12 +5234,12 @@
       <c r="U25" s="13"/>
     </row>
     <row r="26" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="5" t="s">
         <v>12</v>
       </c>
@@ -5233,7 +5256,7 @@
         <v>209</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N26"/>
       <c r="O26"/>
@@ -5244,12 +5267,12 @@
       <c r="U26" s="13"/>
     </row>
     <row r="27" spans="1:21" s="3" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
@@ -5266,7 +5289,7 @@
         <v>209</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N27"/>
       <c r="O27"/>
@@ -5277,20 +5300,20 @@
       <c r="U27" s="13"/>
     </row>
     <row r="28" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35" t="s">
+      <c r="D28" s="43"/>
+      <c r="E28" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="51" t="s">
         <v>183</v>
       </c>
       <c r="G28" s="5" t="s">
@@ -5320,12 +5343,12 @@
       <c r="U28" s="13"/>
     </row>
     <row r="29" spans="1:21" s="3" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
@@ -5351,22 +5374,22 @@
       <c r="U29" s="13"/>
     </row>
     <row r="30" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="51" t="s">
         <v>138</v>
       </c>
       <c r="G30" s="5" t="s">
@@ -5396,12 +5419,12 @@
       <c r="U30" s="16"/>
     </row>
     <row r="31" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="51"/>
       <c r="G31" s="5" t="s">
         <v>12</v>
       </c>
@@ -5418,7 +5441,7 @@
         <v>210</v>
       </c>
       <c r="L31" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N31"/>
       <c r="O31"/>
@@ -5429,12 +5452,12 @@
       <c r="U31" s="16"/>
     </row>
     <row r="32" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="5" t="s">
         <v>12</v>
       </c>
@@ -5451,7 +5474,7 @@
         <v>210</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N32"/>
       <c r="O32"/>
@@ -5462,22 +5485,22 @@
       <c r="U32" s="13"/>
     </row>
     <row r="33" spans="1:21" s="3" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E33" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="38" t="s">
+      <c r="F33" s="50" t="s">
         <v>46</v>
       </c>
       <c r="G33" s="19" t="s">
@@ -5500,12 +5523,12 @@
       <c r="U33" s="13"/>
     </row>
     <row r="34" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="19" t="s">
         <v>12</v>
       </c>
@@ -5526,22 +5549,22 @@
       <c r="U34" s="13"/>
     </row>
     <row r="35" spans="1:21" s="3" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="43" t="s">
         <v>75</v>
       </c>
       <c r="G35" s="5" t="s">
@@ -5572,12 +5595,12 @@
       <c r="U35" s="13"/>
     </row>
     <row r="36" spans="1:21" s="3" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="5" t="s">
         <v>12</v>
       </c>
@@ -5591,7 +5614,7 @@
         <v>21</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>197</v>
@@ -5606,22 +5629,22 @@
       <c r="U36" s="13"/>
     </row>
     <row r="37" spans="1:21" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="43" t="s">
         <v>140</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -5652,12 +5675,12 @@
       <c r="U37" s="13"/>
     </row>
     <row r="38" spans="1:21" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
       <c r="G38" s="5" t="s">
         <v>12</v>
       </c>
@@ -5672,7 +5695,7 @@
       </c>
       <c r="K38" s="26"/>
       <c r="L38" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M38"/>
       <c r="N38"/>
@@ -5684,12 +5707,12 @@
       <c r="U38" s="13"/>
     </row>
     <row r="39" spans="1:21" s="3" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
       <c r="G39" s="5" t="s">
         <v>12</v>
       </c>
@@ -5704,7 +5727,7 @@
       </c>
       <c r="K39" s="26"/>
       <c r="L39" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M39"/>
       <c r="N39"/>
@@ -5752,22 +5775,22 @@
       <c r="U40" s="13"/>
     </row>
     <row r="41" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="43" t="s">
         <v>68</v>
       </c>
       <c r="G41" s="5" t="s">
@@ -5797,12 +5820,12 @@
       <c r="U41" s="13"/>
     </row>
     <row r="42" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
       <c r="G42" s="5" t="s">
         <v>12</v>
       </c>
@@ -5816,10 +5839,10 @@
         <v>21</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L42" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N42"/>
       <c r="O42"/>
@@ -5830,12 +5853,12 @@
       <c r="U42" s="13"/>
     </row>
     <row r="43" spans="1:21" s="3" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
       <c r="G43" s="5" t="s">
         <v>12</v>
       </c>
@@ -5849,10 +5872,10 @@
         <v>22</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N43" s="5"/>
       <c r="O43"/>
@@ -5863,22 +5886,22 @@
       <c r="U43" s="13"/>
     </row>
     <row r="44" spans="1:21" s="3" customFormat="1" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="E44" s="37" t="s">
+      <c r="E44" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="F44" s="35" t="s">
+      <c r="F44" s="43" t="s">
         <v>142</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -5908,12 +5931,12 @@
       <c r="U44" s="13"/>
     </row>
     <row r="45" spans="1:21" s="3" customFormat="1" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="35"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="43"/>
       <c r="G45" s="5" t="s">
         <v>12</v>
       </c>
@@ -5926,11 +5949,11 @@
       <c r="J45" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K45" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="L45" s="50" t="s">
-        <v>237</v>
+      <c r="K45" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="L45" s="33" t="s">
+        <v>236</v>
       </c>
       <c r="N45"/>
       <c r="O45"/>
@@ -5941,12 +5964,12 @@
       <c r="U45" s="13"/>
     </row>
     <row r="46" spans="1:21" s="3" customFormat="1" ht="108.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
       <c r="G46" s="5" t="s">
         <v>12</v>
       </c>
@@ -5959,11 +5982,11 @@
       <c r="J46" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K46" s="50" t="s">
-        <v>207</v>
+      <c r="K46" s="57" t="s">
+        <v>258</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N46"/>
       <c r="O46"/>
@@ -5974,34 +5997,34 @@
       <c r="U46" s="13"/>
     </row>
     <row r="47" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="F47" s="34" t="s">
+      <c r="F47" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="52" t="s">
+      <c r="G47" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="52" t="s">
+      <c r="H47" s="35" t="s">
         <v>16</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J47" s="52" t="s">
+      <c r="J47" s="35" t="s">
         <v>20</v>
       </c>
       <c r="K47"/>
@@ -6017,22 +6040,22 @@
       <c r="U47" s="13"/>
     </row>
     <row r="48" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="52" t="s">
+      <c r="A48" s="52"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="52" t="s">
+      <c r="H48" s="35" t="s">
         <v>18</v>
       </c>
       <c r="I48" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J48" s="52" t="s">
+      <c r="J48" s="35" t="s">
         <v>21</v>
       </c>
       <c r="K48"/>
@@ -6153,22 +6176,22 @@
       <c r="U51" s="13"/>
     </row>
     <row r="52" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="38" t="s">
+      <c r="D52" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="38" t="s">
+      <c r="E52" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="F52" s="38" t="s">
+      <c r="F52" s="50" t="s">
         <v>124</v>
       </c>
       <c r="G52" s="5"/>
@@ -6188,12 +6211,12 @@
       <c r="U52" s="13"/>
     </row>
     <row r="53" spans="1:21" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -6240,22 +6263,22 @@
       <c r="U54" s="13"/>
     </row>
     <row r="55" spans="1:21" s="3" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D55" s="35" t="s">
+      <c r="D55" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="E55" s="35" t="s">
+      <c r="E55" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="F55" s="43" t="s">
         <v>144</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -6285,12 +6308,12 @@
       <c r="U55" s="15"/>
     </row>
     <row r="56" spans="1:21" s="3" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
       <c r="G56" s="5" t="s">
         <v>12</v>
       </c>
@@ -6316,22 +6339,22 @@
       <c r="U56" s="13"/>
     </row>
     <row r="57" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="35" t="s">
+      <c r="D57" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E57" s="35" t="s">
+      <c r="E57" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="35" t="s">
+      <c r="F57" s="43" t="s">
         <v>109</v>
       </c>
       <c r="G57" s="5" t="s">
@@ -6361,12 +6384,12 @@
       <c r="U57" s="13"/>
     </row>
     <row r="58" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="35"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
@@ -6382,12 +6405,12 @@
       <c r="U58" s="13"/>
     </row>
     <row r="59" spans="1:21" s="3" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
       <c r="G59" s="5" t="s">
         <v>12</v>
       </c>
@@ -6401,8 +6424,8 @@
         <v>21</v>
       </c>
       <c r="K59" s="5"/>
-      <c r="L59" s="50" t="s">
-        <v>238</v>
+      <c r="L59" s="33" t="s">
+        <v>237</v>
       </c>
       <c r="N59"/>
       <c r="O59"/>
@@ -6413,12 +6436,12 @@
       <c r="U59" s="13"/>
     </row>
     <row r="60" spans="1:21" s="3" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
       <c r="G60" s="5" t="s">
         <v>12</v>
       </c>
@@ -6433,7 +6456,7 @@
       </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N60"/>
       <c r="O60"/>
@@ -6444,22 +6467,22 @@
       <c r="U60" s="13"/>
     </row>
     <row r="61" spans="1:21" s="3" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E61" s="35" t="s">
+      <c r="E61" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="F61" s="35" t="s">
+      <c r="F61" s="43" t="s">
         <v>146</v>
       </c>
       <c r="G61" s="5" t="s">
@@ -6489,12 +6512,12 @@
       <c r="U61" s="13"/>
     </row>
     <row r="62" spans="1:21" s="3" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
       <c r="G62" s="5" t="s">
         <v>12</v>
       </c>
@@ -6508,8 +6531,8 @@
         <v>21</v>
       </c>
       <c r="K62" s="5"/>
-      <c r="L62" s="50" t="s">
-        <v>243</v>
+      <c r="L62" s="33" t="s">
+        <v>242</v>
       </c>
       <c r="N62"/>
       <c r="O62"/>
@@ -6520,12 +6543,12 @@
       <c r="U62" s="13"/>
     </row>
     <row r="63" spans="1:21" s="3" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
       <c r="G63" s="5" t="s">
         <v>12</v>
       </c>
@@ -6540,7 +6563,7 @@
       </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N63"/>
       <c r="O63"/>
@@ -6551,22 +6574,22 @@
       <c r="U63" s="13"/>
     </row>
     <row r="64" spans="1:21" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="D64" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E64" s="35" t="s">
+      <c r="E64" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F64" s="35" t="s">
+      <c r="F64" s="43" t="s">
         <v>100</v>
       </c>
       <c r="G64" s="5" t="s">
@@ -6596,12 +6619,12 @@
       <c r="U64" s="13"/>
     </row>
     <row r="65" spans="1:21" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
       <c r="G65" s="5" t="s">
         <v>12</v>
       </c>
@@ -6615,10 +6638,10 @@
         <v>21</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L65" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N65"/>
       <c r="O65"/>
@@ -6629,12 +6652,12 @@
       <c r="U65" s="13"/>
     </row>
     <row r="66" spans="1:21" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
       <c r="G66" s="5" t="s">
         <v>12</v>
       </c>
@@ -6648,10 +6671,10 @@
         <v>22</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N66"/>
       <c r="O66"/>
@@ -6662,22 +6685,22 @@
       <c r="U66" s="13"/>
     </row>
     <row r="67" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="38" t="s">
+      <c r="C67" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D67" s="38" t="s">
+      <c r="D67" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="38" t="s">
+      <c r="E67" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="38" t="s">
+      <c r="F67" s="50" t="s">
         <v>99</v>
       </c>
       <c r="G67" s="19" t="s">
@@ -6699,12 +6722,12 @@
       <c r="U67" s="13"/>
     </row>
     <row r="68" spans="1:21" s="3" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
       <c r="G68" s="19" t="s">
         <v>12</v>
       </c>
@@ -6724,23 +6747,23 @@
       <c r="U68" s="13"/>
     </row>
     <row r="69" spans="1:21" s="3" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="35" t="s">
+      <c r="C69" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D69" s="35" t="s">
+      <c r="D69" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="35" t="s">
+      <c r="E69" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F69" s="35" t="s">
-        <v>213</v>
+      <c r="F69" s="43" t="s">
+        <v>212</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>10</v>
@@ -6768,13 +6791,13 @@
       <c r="S69"/>
       <c r="U69" s="13"/>
     </row>
-    <row r="70" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
+    <row r="70" spans="1:21" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
       <c r="G70" s="5" t="s">
         <v>12</v>
       </c>
@@ -6788,7 +6811,7 @@
         <v>21</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L70" s="5" t="s">
         <v>200</v>
@@ -6802,22 +6825,22 @@
       <c r="U70" s="13"/>
     </row>
     <row r="71" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="35" t="s">
+      <c r="C71" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="35" t="s">
+      <c r="D71" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="35" t="s">
+      <c r="E71" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="F71" s="35" t="s">
+      <c r="F71" s="43" t="s">
         <v>101</v>
       </c>
       <c r="G71" s="5" t="s">
@@ -6847,12 +6870,12 @@
       <c r="U71" s="5"/>
     </row>
     <row r="72" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
       <c r="G72" s="5" t="s">
         <v>12</v>
       </c>
@@ -6866,10 +6889,10 @@
         <v>21</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L72" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N72"/>
       <c r="O72"/>
@@ -6879,13 +6902,13 @@
       <c r="S72"/>
       <c r="U72" s="5"/>
     </row>
-    <row r="73" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
+    <row r="73" spans="1:21" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
       <c r="G73" s="5" t="s">
         <v>12</v>
       </c>
@@ -6899,10 +6922,10 @@
         <v>22</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N73"/>
       <c r="O73"/>
@@ -6913,22 +6936,22 @@
       <c r="U73" s="13"/>
     </row>
     <row r="74" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="C74" s="35" t="s">
+      <c r="C74" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D74" s="35" t="s">
+      <c r="D74" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E74" s="35" t="s">
+      <c r="E74" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="F74" s="35" t="s">
+      <c r="F74" s="43" t="s">
         <v>102</v>
       </c>
       <c r="G74" s="5" t="s">
@@ -6958,12 +6981,12 @@
       <c r="U74" s="13"/>
     </row>
     <row r="75" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
       <c r="G75" s="5" t="s">
         <v>12</v>
       </c>
@@ -6977,8 +7000,8 @@
         <v>21</v>
       </c>
       <c r="K75" s="5"/>
-      <c r="L75" s="50" t="s">
-        <v>247</v>
+      <c r="L75" s="33" t="s">
+        <v>246</v>
       </c>
       <c r="N75"/>
       <c r="O75"/>
@@ -6989,12 +7012,12 @@
       <c r="U75" s="13"/>
     </row>
     <row r="76" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="35"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
       <c r="G76" s="5" t="s">
         <v>12</v>
       </c>
@@ -7009,7 +7032,7 @@
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N76"/>
       <c r="O76"/>
@@ -7020,22 +7043,22 @@
       <c r="U76" s="13"/>
     </row>
     <row r="77" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="35" t="s">
+      <c r="C77" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D77" s="42" t="s">
+      <c r="D77" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="E77" s="35" t="s">
+      <c r="E77" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="F77" s="35" t="s">
+      <c r="F77" s="43" t="s">
         <v>106</v>
       </c>
       <c r="G77" s="5" t="s">
@@ -7065,12 +7088,12 @@
       <c r="U77" s="13"/>
     </row>
     <row r="78" spans="1:21" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="35"/>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="49"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
       <c r="G78" s="5" t="s">
         <v>12</v>
       </c>
@@ -7084,8 +7107,8 @@
         <v>21</v>
       </c>
       <c r="K78" s="5"/>
-      <c r="L78" s="50" t="s">
-        <v>249</v>
+      <c r="L78" s="33" t="s">
+        <v>248</v>
       </c>
       <c r="N78"/>
       <c r="O78"/>
@@ -7096,12 +7119,12 @@
       <c r="U78" s="13"/>
     </row>
     <row r="79" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="35"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
+      <c r="A79" s="43"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="49"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
       <c r="G79" s="5" t="s">
         <v>12</v>
       </c>
@@ -7116,7 +7139,7 @@
       </c>
       <c r="K79" s="5"/>
       <c r="L79" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N79"/>
       <c r="O79"/>
@@ -7127,22 +7150,22 @@
       <c r="U79" s="13"/>
     </row>
     <row r="80" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="35" t="s">
+      <c r="C80" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D80" s="42" t="s">
+      <c r="D80" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="E80" s="35" t="s">
+      <c r="E80" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="F80" s="35" t="s">
+      <c r="F80" s="43" t="s">
         <v>107</v>
       </c>
       <c r="G80" s="5" t="s">
@@ -7172,12 +7195,12 @@
       <c r="U80" s="13"/>
     </row>
     <row r="81" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="35"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="35"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35"/>
+      <c r="A81" s="43"/>
+      <c r="B81" s="43"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="49"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
       <c r="G81" s="5" t="s">
         <v>12</v>
       </c>
@@ -7190,11 +7213,11 @@
       <c r="J81" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K81" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="L81" s="50" t="s">
-        <v>249</v>
+      <c r="K81" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="L81" s="33" t="s">
+        <v>248</v>
       </c>
       <c r="N81"/>
       <c r="O81"/>
@@ -7205,12 +7228,12 @@
       <c r="U81" s="13"/>
     </row>
     <row r="82" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="35"/>
-      <c r="B82" s="35"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
       <c r="G82" s="5" t="s">
         <v>12</v>
       </c>
@@ -7223,11 +7246,11 @@
       <c r="J82" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K82" s="50" t="s">
-        <v>253</v>
+      <c r="K82" s="33" t="s">
+        <v>251</v>
       </c>
       <c r="L82" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N82"/>
       <c r="O82"/>
@@ -7269,18 +7292,18 @@
       <c r="S83"/>
     </row>
     <row r="84" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
-      <c r="B84" s="47"/>
-      <c r="C84" s="43" t="s">
+      <c r="A84" s="40"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="D84" s="43" t="s">
+      <c r="D84" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="E84" s="43" t="s">
+      <c r="E84" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="F84" s="43" t="s">
+      <c r="F84" s="41" t="s">
         <v>153</v>
       </c>
       <c r="G84" s="5" t="s">
@@ -7303,12 +7326,12 @@
       <c r="S84"/>
     </row>
     <row r="85" spans="1:21" s="3" customFormat="1" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
-      <c r="B85" s="47"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="40"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="41"/>
+      <c r="E85" s="41"/>
+      <c r="F85" s="41"/>
       <c r="G85" s="5" t="s">
         <v>12</v>
       </c>
@@ -7329,18 +7352,18 @@
       <c r="S85"/>
     </row>
     <row r="86" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="47"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="43" t="s">
+      <c r="A86" s="40"/>
+      <c r="B86" s="40"/>
+      <c r="C86" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="D86" s="43" t="s">
+      <c r="D86" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="E86" s="43" t="s">
+      <c r="E86" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="F86" s="43" t="s">
+      <c r="F86" s="41" t="s">
         <v>155</v>
       </c>
       <c r="G86" s="5" t="s">
@@ -7363,12 +7386,12 @@
       <c r="S86"/>
     </row>
     <row r="87" spans="1:21" s="3" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="47"/>
-      <c r="B87" s="47"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="41"/>
+      <c r="F87" s="41"/>
       <c r="G87" s="5" t="s">
         <v>12</v>
       </c>
@@ -7389,22 +7412,22 @@
       <c r="S87"/>
     </row>
     <row r="88" spans="1:21" s="3" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="43" t="s">
+      <c r="A88" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B88" s="43" t="s">
+      <c r="B88" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C88" s="43" t="s">
+      <c r="C88" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="D88" s="43" t="s">
+      <c r="D88" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E88" s="43" t="s">
+      <c r="E88" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="F88" s="43" t="s">
+      <c r="F88" s="41" t="s">
         <v>158</v>
       </c>
       <c r="G88" s="5" t="s">
@@ -7432,13 +7455,13 @@
       <c r="R88"/>
       <c r="S88"/>
     </row>
-    <row r="89" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="43"/>
-      <c r="B89" s="47"/>
-      <c r="C89" s="43"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43"/>
+    <row r="89" spans="1:21" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="41"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="41"/>
+      <c r="F89" s="41"/>
       <c r="G89" s="5" t="s">
         <v>12</v>
       </c>
@@ -7451,8 +7474,8 @@
       <c r="J89" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K89" s="3" t="s">
-        <v>251</v>
+      <c r="K89" s="22" t="s">
+        <v>256</v>
       </c>
       <c r="L89" s="3" t="s">
         <v>201</v>
@@ -7465,12 +7488,12 @@
       <c r="S89"/>
     </row>
     <row r="90" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="43"/>
-      <c r="E90" s="43"/>
-      <c r="F90" s="49" t="s">
+      <c r="A90" s="40"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="41"/>
+      <c r="D90" s="41"/>
+      <c r="E90" s="41"/>
+      <c r="F90" s="42" t="s">
         <v>159</v>
       </c>
       <c r="G90" s="5" t="s">
@@ -7499,12 +7522,12 @@
       <c r="S90"/>
     </row>
     <row r="91" spans="1:21" s="3" customFormat="1" ht="87.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="47"/>
-      <c r="B91" s="47"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="49"/>
+      <c r="A91" s="40"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="41"/>
+      <c r="E91" s="41"/>
+      <c r="F91" s="42"/>
       <c r="G91" s="5" t="s">
         <v>12</v>
       </c>
@@ -7518,7 +7541,7 @@
         <v>21</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L91" s="22" t="s">
         <v>202</v>
@@ -7531,11 +7554,11 @@
       <c r="S91"/>
     </row>
     <row r="92" spans="1:21" s="3" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C92" s="51" t="s">
+      <c r="C92" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="D92" s="51"/>
-      <c r="E92" s="51" t="s">
+      <c r="D92" s="34"/>
+      <c r="E92" s="34" t="s">
         <v>161</v>
       </c>
       <c r="F92" s="29" t="s">
@@ -7548,11 +7571,11 @@
         <v>16</v>
       </c>
       <c r="I92" s="19"/>
-      <c r="J92" s="53" t="s">
+      <c r="J92" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="K92" s="54"/>
-      <c r="L92" s="55" t="s">
+      <c r="K92" s="37"/>
+      <c r="L92" s="38" t="s">
         <v>170</v>
       </c>
       <c r="N92"/>
@@ -7563,12 +7586,12 @@
       <c r="S92"/>
     </row>
     <row r="93" spans="1:21" s="3" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
-      <c r="B93" s="47"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="48" t="s">
+      <c r="A93" s="40"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="41"/>
+      <c r="D93" s="41"/>
+      <c r="E93" s="41"/>
+      <c r="F93" s="39" t="s">
         <v>115</v>
       </c>
       <c r="G93" s="5" t="s">
@@ -7597,12 +7620,12 @@
       <c r="S93"/>
     </row>
     <row r="94" spans="1:21" s="3" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
-      <c r="B94" s="47"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
-      <c r="F94" s="48"/>
+      <c r="A94" s="40"/>
+      <c r="B94" s="40"/>
+      <c r="C94" s="41"/>
+      <c r="D94" s="41"/>
+      <c r="E94" s="41"/>
+      <c r="F94" s="39"/>
       <c r="G94" s="5" t="s">
         <v>12</v>
       </c>
@@ -7684,24 +7707,24 @@
       <c r="U96" s="13"/>
     </row>
     <row r="97" spans="1:21" s="3" customFormat="1" ht="107.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="40"/>
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="41" t="s">
+      <c r="A97" s="47"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="F97" s="40"/>
-      <c r="G97" s="52" t="s">
+      <c r="F97" s="47"/>
+      <c r="G97" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H97" s="52" t="s">
+      <c r="H97" s="35" t="s">
         <v>16</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J97" s="52" t="s">
+      <c r="J97" s="35" t="s">
         <v>20</v>
       </c>
       <c r="K97" t="s">
@@ -7719,22 +7742,22 @@
       <c r="U97" s="15"/>
     </row>
     <row r="98" spans="1:21" s="3" customFormat="1" ht="107.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="40"/>
-      <c r="B98" s="40"/>
-      <c r="C98" s="40"/>
-      <c r="D98" s="40"/>
-      <c r="E98" s="41"/>
-      <c r="F98" s="40"/>
-      <c r="G98" s="52" t="s">
+      <c r="A98" s="47"/>
+      <c r="B98" s="47"/>
+      <c r="C98" s="47"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="48"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H98" s="52" t="s">
+      <c r="H98" s="35" t="s">
         <v>18</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J98" s="52" t="s">
+      <c r="J98" s="35" t="s">
         <v>21</v>
       </c>
       <c r="K98"/>
@@ -7750,30 +7773,30 @@
       <c r="U98" s="15"/>
     </row>
     <row r="99" spans="1:21" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A99" s="33"/>
-      <c r="B99" s="33"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="34" t="s">
+      <c r="A99" s="52"/>
+      <c r="B99" s="52"/>
+      <c r="C99" s="52"/>
+      <c r="D99" s="52"/>
+      <c r="E99" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="F99" s="34" t="s">
+      <c r="F99" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="G99" s="52" t="s">
+      <c r="G99" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H99" s="52" t="s">
+      <c r="H99" s="35" t="s">
         <v>16</v>
       </c>
       <c r="I99" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J99" s="52" t="s">
+      <c r="J99" s="35" t="s">
         <v>20</v>
       </c>
       <c r="K99" s="25" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L99" s="31" t="s">
         <v>176</v>
@@ -7786,27 +7809,27 @@
       <c r="S99"/>
       <c r="U99" s="13"/>
     </row>
-    <row r="100" spans="1:21" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="33"/>
-      <c r="B100" s="33"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="34"/>
-      <c r="F100" s="34"/>
-      <c r="G100" s="52" t="s">
+    <row r="100" spans="1:21" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A100" s="52"/>
+      <c r="B100" s="52"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="53"/>
+      <c r="F100" s="53"/>
+      <c r="G100" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H100" s="52" t="s">
+      <c r="H100" s="35" t="s">
         <v>18</v>
       </c>
       <c r="I100" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J100" s="52" t="s">
+      <c r="J100" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K100" s="25" t="s">
-        <v>211</v>
+      <c r="K100" s="56" t="s">
+        <v>255</v>
       </c>
       <c r="L100" s="25" t="s">
         <v>205</v>
@@ -7829,21 +7852,21 @@
         <v>185</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F101" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="G101" s="52" t="s">
+      <c r="G101" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H101" s="52" t="s">
+      <c r="H101" s="35" t="s">
         <v>16</v>
       </c>
       <c r="I101" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="J101" s="52" t="s">
+      <c r="J101" s="35" t="s">
         <v>20</v>
       </c>
       <c r="K101" t="s">
@@ -7867,10 +7890,10 @@
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
-      <c r="G102" s="52"/>
-      <c r="H102" s="52"/>
+      <c r="G102" s="35"/>
+      <c r="H102" s="35"/>
       <c r="I102"/>
-      <c r="J102" s="52"/>
+      <c r="J102" s="35"/>
       <c r="K102"/>
       <c r="L102"/>
       <c r="N102"/>
@@ -7888,10 +7911,10 @@
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
-      <c r="G103" s="52"/>
-      <c r="H103" s="52"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="35"/>
       <c r="I103"/>
-      <c r="J103" s="52"/>
+      <c r="J103" s="35"/>
       <c r="K103"/>
       <c r="L103"/>
       <c r="N103"/>
@@ -7909,10 +7932,10 @@
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
-      <c r="G104" s="52"/>
-      <c r="H104" s="52"/>
+      <c r="G104" s="35"/>
+      <c r="H104" s="35"/>
       <c r="I104"/>
-      <c r="J104" s="52"/>
+      <c r="J104" s="35"/>
       <c r="K104"/>
       <c r="L104"/>
       <c r="N104"/>
@@ -7930,10 +7953,10 @@
       <c r="D105"/>
       <c r="E105"/>
       <c r="F105"/>
-      <c r="G105" s="52"/>
-      <c r="H105" s="52"/>
+      <c r="G105" s="35"/>
+      <c r="H105" s="35"/>
       <c r="I105"/>
-      <c r="J105" s="52"/>
+      <c r="J105" s="35"/>
       <c r="K105" s="32"/>
       <c r="L105"/>
       <c r="N105"/>
@@ -7951,10 +7974,10 @@
       <c r="D106"/>
       <c r="E106"/>
       <c r="F106"/>
-      <c r="G106" s="52"/>
-      <c r="H106" s="52"/>
+      <c r="G106" s="35"/>
+      <c r="H106" s="35"/>
       <c r="I106"/>
-      <c r="J106" s="52"/>
+      <c r="J106" s="35"/>
       <c r="K106" s="32"/>
       <c r="M106"/>
       <c r="N106"/>
@@ -9471,19 +9494,19 @@
     </row>
     <row r="132" spans="1:1036" x14ac:dyDescent="0.25">
       <c r="A132" s="17"/>
-      <c r="B132" s="36" t="s">
+      <c r="B132" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C132" s="36"/>
-      <c r="D132" s="36"/>
-      <c r="E132" s="36"/>
-      <c r="F132" s="36"/>
-      <c r="G132" s="36"/>
-      <c r="H132" s="36"/>
-      <c r="I132" s="36"/>
-      <c r="J132" s="36"/>
-      <c r="K132" s="36"/>
-      <c r="L132" s="36"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="55"/>
+      <c r="E132" s="55"/>
+      <c r="F132" s="55"/>
+      <c r="G132" s="55"/>
+      <c r="H132" s="55"/>
+      <c r="I132" s="55"/>
+      <c r="J132" s="55"/>
+      <c r="K132" s="55"/>
+      <c r="L132" s="55"/>
       <c r="M132" s="3"/>
       <c r="T132" s="3"/>
     </row>
@@ -9507,36 +9530,163 @@
     </row>
   </sheetData>
   <mergeCells count="211">
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="E99:E100"/>
+    <mergeCell ref="F99:F100"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="B132:L132"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="D77:D79"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="F77:F79"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -9561,177 +9711,38 @@
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="E80:E82"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="D77:D79"/>
-    <mergeCell ref="E77:E79"/>
-    <mergeCell ref="F77:F79"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="B132:L132"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="E99:E100"/>
-    <mergeCell ref="F99:F100"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
-  <conditionalFormatting sqref="M41:M42 M5">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="100"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
+  <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="M2:M3 M7:M8 M13:M14 M16:M17 M22:M23 M25:M26 M28 M30:M31 M33 M35 M37:M39 M44:M45 M49 M51 M63 M66 M68 M70 M73 M76 M79 M82 M96:M97 M101 M103 M105 L107 M109">
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -9768,7 +9779,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M84 M86 M88 M90 M92">
+  <conditionalFormatting sqref="M41:M42 M5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M86 M84 M88 M90 M92">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -9785,7 +9808,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$8</xm:f>

</xml_diff>